<commit_message>
colocando referencias no excel
</commit_message>
<xml_diff>
--- a/referencias_extras.xlsx
+++ b/referencias_extras.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william/Documents/curso-r/CursoRutils/inst/minimal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william/Documents/curso-r/202105-dashboards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71D2336-605E-CC42-AD04-40BFC18A71B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F1E491-5B7F-1F4C-93EB-E9B79C8D1BB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39920" yWindow="-100" windowWidth="27500" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="54140" yWindow="1100" windowWidth="24820" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>aula</t>
   </si>
@@ -32,6 +32,36 @@
   </si>
   <si>
     <t>url</t>
+  </si>
+  <si>
+    <t>Material extra</t>
+  </si>
+  <si>
+    <t>Caixas de diálogo no Shiny</t>
+  </si>
+  <si>
+    <t>https://shiny.rstudio.com/articles/modal-dialogs.html</t>
+  </si>
+  <si>
+    <t>Pacote fresh</t>
+  </si>
+  <si>
+    <t>https://github.com/dreamRs/fresh</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=s9GKim52E4k</t>
+  </si>
+  <si>
+    <t>Vídeo: Shinydashboard, pacote fresh e CSS</t>
+  </si>
+  <si>
+    <t>Live sobre módulos</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=xp5aMvwqEMY&amp;ab_channel=Curso-R</t>
+  </si>
+  <si>
+    <t>Material Extra</t>
   </si>
 </sst>
 </file>
@@ -46,25 +76,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="10"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -72,156 +97,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1382,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1398,382 +1281,113 @@
     <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+    <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+    <row r="3" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+    <row r="4" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+    <row r="5" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="8"/>
-    </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="4"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="12"/>
-    </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="4"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="12"/>
-    </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="14"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="12"/>
-    </row>
-    <row r="44" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="17"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="12"/>
-    </row>
-    <row r="45" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="17"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="12"/>
-    </row>
-    <row r="46" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="18"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="22"/>
-    </row>
+    <row r="6" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>